<commit_message>
Add config files that work with current database contents
</commit_message>
<xml_diff>
--- a/example-config.xlsx
+++ b/example-config.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="assets" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="baselines" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="congestion" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="assets" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="baselines" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -30,7 +37,7 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">typical-day</t>
+    <t xml:space="preserve">typical_day</t>
   </si>
   <si>
     <t xml:space="preserve">group</t>
@@ -67,26 +74,23 @@
   </si>
   <si>
     <t xml:space="preserve">sjv2500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTU1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTU2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -104,31 +108,24 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="13.95"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,8 +170,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,19 +206,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>80280</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="0" name="Text Frame 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="510840" y="349200"/>
-          <a:ext cx="5258880" cy="3462120"/>
+          <a:ext cx="5267520" cy="3461760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -225,90 +230,90 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Excel configuration file for the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>flex metrics tool</a:t>
+            <a:t>Excel configuration file for the flex metrics tool</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>In the ‘assets’ sheet, you provide how </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>many devices of the device types that </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>the flex metrics tool support are </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>present in the scenario.</a:t>
+            <a:t>In the ‘assets’ sheet, you provide how many devices of the device types are present in the scenario.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Run the flex metrics database </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>exploration tool to find out which </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>devices are supported:</a:t>
+            <a:t>Run the flex metrics database exploration tool to find out which devices are supported:</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:latin typeface="Courier New"/>
@@ -320,40 +325,26 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Please not that for all devices you </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>provide in the ‘amount’ column the </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>number of devices of that type and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>for that group but for PV you provide </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>the peak power in Watt. </a:t>
+            <a:t>NOTE: for all devices the ‘amount’ column contains the number of devices of that type and group but for PV it contains the peak power in Watt. </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -373,11 +364,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -395,118 +386,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.22"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>9722</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B2" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -525,28 +426,298 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.22"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>9722</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>0.760416666666667</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>0.770833333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>0.791666666666666</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>0.802083333333333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>0.822916666666666</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>0.833333333333333</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>0.854166666666666</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>0.864583333333333</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>0.874999999999999</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>0.885416666666666</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>0.895833333333332</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>0.906249999999999</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>0.916666666666666</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>0.927083333333332</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
+        <v>0.937499999999999</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>0.947916666666665</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>0.958333333333332</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>0.968749999999999</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>0.979166666666665</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
+        <v>0.989583333333332</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
+        <v>1.01041666666667</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
+        <v>1.02083333333333</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="n">
+        <v>1.03125</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="n">
+        <v>1.04166666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>